<commit_message>
Gathered all base model results.
</commit_message>
<xml_diff>
--- a/Results/kNN.xlsx
+++ b/Results/kNN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/kbh15_ic_ac_uk/Documents/University/Course/4th Year/Autumn/EE4-68 Pattern Recognition/Coursework 2018/Coursework 2/EE4-68_PR_CW_2/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{973D0D37-EE25-4F8A-B326-65CA8CCE1C7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FC9333E-8FB3-4377-A801-18C1D2686840}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12458" xr2:uid="{5AEE031F-43BD-408F-A6DA-9B6C39BA7A46}"/>
   </bookViews>
@@ -25,15 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Euclidian</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Chebyshev</t>
   </si>
   <si>
     <t>City Block</t>
+  </si>
+  <si>
+    <t>Standardised Euclidean</t>
+  </si>
+  <si>
+    <t>Euclidean</t>
+  </si>
+  <si>
+    <t>Metric vs K</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -41,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -78,17 +111,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -99,6 +140,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DBC49BE3-4983-460A-9C3B-3F4CC6EE95F9}" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:J5" xr:uid="{E469B231-6136-4F15-9BE2-20070ED13C69}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{3AE171A5-244F-4974-8DD8-3FABAE35225E}" name="Metric vs K"/>
+    <tableColumn id="2" xr3:uid="{60C9AA2F-A2A9-496C-A2F1-A41517901F5A}" name="1"/>
+    <tableColumn id="3" xr3:uid="{F1608E6F-8801-4A4D-A362-5E522306E676}" name="2"/>
+    <tableColumn id="4" xr3:uid="{C631C08A-618E-4DF2-B2E6-EBD77829076E}" name="3"/>
+    <tableColumn id="5" xr3:uid="{A5F955A0-C562-4424-82F6-BD9AFBE7AECB}" name="5"/>
+    <tableColumn id="6" xr3:uid="{8DBF8918-9A16-4C1A-BA1B-4A20FD7DF1E7}" name="10"/>
+    <tableColumn id="7" xr3:uid="{F2EDF611-06E3-4A20-B0AC-93556E3DEA72}" name="20"/>
+    <tableColumn id="8" xr3:uid="{620219BD-7A2F-4BF3-BE1D-E052DAB8D389}" name="50"/>
+    <tableColumn id="9" xr3:uid="{C229E30E-DFFB-4859-BEA4-9A015370BDD3}" name="75"/>
+    <tableColumn id="10" xr3:uid="{6298ACCA-ACC8-456E-9287-223C2F4DD639}" name="100" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -398,51 +458,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735AB61D-882E-4A72-BED5-7895F88B9249}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="7" width="9.06640625" style="1"/>
-    <col min="8" max="9" width="9.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1">
+      <c r="C1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1">
-        <v>50</v>
-      </c>
-      <c r="I1" s="1">
-        <v>75</v>
-      </c>
-      <c r="J1" s="1">
-        <v>100</v>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2">
         <v>0.47</v>
@@ -474,7 +539,7 @@
     </row>
     <row r="3" spans="1:10" ht="14.65" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2">
         <v>0.34285714285714203</v>
@@ -506,7 +571,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>0.47214285714285698</v>
@@ -534,10 +599,45 @@
       </c>
       <c r="J4" s="1">
         <v>0.94571428571428495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.46857142857142797</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.53714285714285703</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.65785714285714203</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.73785714285714199</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.81357142857142795</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.88428571428571401</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.91928571428571404</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.94</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added pca and lad results (without standardisation)
</commit_message>
<xml_diff>
--- a/Results/kNN.xlsx
+++ b/Results/kNN.xlsx
@@ -1,22 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/kbh15_ic_ac_uk/Documents/University/Course/4th Year/Autumn/EE4-68 Pattern Recognition/Coursework 2018/Coursework 2/EE4-68_PR_CW_2/Results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FC9333E-8FB3-4377-A801-18C1D2686840}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="12458" xr2:uid="{5AEE031F-43BD-408F-A6DA-9B6C39BA7A46}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12460"/>
   </bookViews>
   <sheets>
     <sheet name="kNN" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Chebyshev</t>
   </si>
@@ -67,16 +64,25 @@
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>Mpca vs K</t>
+  </si>
+  <si>
+    <t>Mlda vs K</t>
+  </si>
+  <si>
+    <t>cum_explained var</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,16 +96,46 @@
       <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -107,27 +143,107 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -143,19 +259,65 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DBC49BE3-4983-460A-9C3B-3F4CC6EE95F9}" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:J5" xr:uid="{E469B231-6136-4F15-9BE2-20070ED13C69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A1:J5"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{3AE171A5-244F-4974-8DD8-3FABAE35225E}" name="Metric vs K"/>
-    <tableColumn id="2" xr3:uid="{60C9AA2F-A2A9-496C-A2F1-A41517901F5A}" name="1"/>
-    <tableColumn id="3" xr3:uid="{F1608E6F-8801-4A4D-A362-5E522306E676}" name="2"/>
-    <tableColumn id="4" xr3:uid="{C631C08A-618E-4DF2-B2E6-EBD77829076E}" name="3"/>
-    <tableColumn id="5" xr3:uid="{A5F955A0-C562-4424-82F6-BD9AFBE7AECB}" name="5"/>
-    <tableColumn id="6" xr3:uid="{8DBF8918-9A16-4C1A-BA1B-4A20FD7DF1E7}" name="10"/>
-    <tableColumn id="7" xr3:uid="{F2EDF611-06E3-4A20-B0AC-93556E3DEA72}" name="20"/>
-    <tableColumn id="8" xr3:uid="{620219BD-7A2F-4BF3-BE1D-E052DAB8D389}" name="50"/>
-    <tableColumn id="9" xr3:uid="{C229E30E-DFFB-4859-BEA4-9A015370BDD3}" name="75"/>
-    <tableColumn id="10" xr3:uid="{6298ACCA-ACC8-456E-9287-223C2F4DD639}" name="100" dataDxfId="1"/>
+    <tableColumn id="1" name="Metric vs K" dataDxfId="12"/>
+    <tableColumn id="2" name="1"/>
+    <tableColumn id="3" name="2"/>
+    <tableColumn id="4" name="3"/>
+    <tableColumn id="5" name="5"/>
+    <tableColumn id="6" name="10"/>
+    <tableColumn id="7" name="20"/>
+    <tableColumn id="8" name="50"/>
+    <tableColumn id="9" name="75"/>
+    <tableColumn id="10" name="100" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K12" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A8:K12"/>
+  <sortState ref="A9:K12">
+    <sortCondition ref="A8:A12"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Mpca vs K" dataDxfId="11"/>
+    <tableColumn id="2" name="1"/>
+    <tableColumn id="3" name="2"/>
+    <tableColumn id="4" name="3"/>
+    <tableColumn id="5" name="5"/>
+    <tableColumn id="6" name="10"/>
+    <tableColumn id="7" name="20"/>
+    <tableColumn id="8" name="50"/>
+    <tableColumn id="9" name="75"/>
+    <tableColumn id="10" name="100" dataDxfId="15"/>
+    <tableColumn id="11" name="cum_explained var"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A14:K18" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A14:K18"/>
+  <sortState ref="A15:K18">
+    <sortCondition ref="A14:A18"/>
+  </sortState>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Mlda vs K" dataDxfId="10"/>
+    <tableColumn id="2" name="1" dataDxfId="9"/>
+    <tableColumn id="3" name="2" dataDxfId="8"/>
+    <tableColumn id="4" name="3" dataDxfId="7"/>
+    <tableColumn id="5" name="5" dataDxfId="6"/>
+    <tableColumn id="6" name="10" dataDxfId="5"/>
+    <tableColumn id="7" name="20" dataDxfId="4"/>
+    <tableColumn id="8" name="50" dataDxfId="3"/>
+    <tableColumn id="9" name="75" dataDxfId="2"/>
+    <tableColumn id="10" name="100" dataDxfId="1"/>
+    <tableColumn id="11" name="cum_explained var" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -204,7 +366,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -256,7 +418,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -450,31 +612,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735AB61D-882E-4A72-BED5-7895F88B9249}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -505,8 +667,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="15">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2">
@@ -537,8 +699,8 @@
         <v>0.94571428571428495</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" ht="15">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2">
@@ -569,8 +731,8 @@
         <v>0.84285714285714197</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1">
@@ -601,8 +763,8 @@
         <v>0.94571428571428495</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1">
@@ -633,11 +795,368 @@
         <v>0.94</v>
       </c>
     </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="5">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.46785714285714203</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.54571428571428504</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.59571428571428497</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.67571428571428505</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.748571428571428</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.82571428571428496</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.89785714285714202</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.93214285714285705</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.94571428571428495</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.92917554909895905</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="5">
+        <v>200</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.46928571428571397</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.67357142857142804</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.82857142857142796</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.89857142857142802</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.93214285714285705</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.94499999999999995</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.96531732391257996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="5">
+        <v>300</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.46857142857142797</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.54642857142857104</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.59428571428571397</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.67285714285714204</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.749285714285714</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.89714285714285702</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.93214285714285705</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.94571428571428495</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.97863739074901601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="5">
+        <v>350</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.46642857142857103</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.54857142857142804</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.59428571428571397</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.67285714285714204</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.748571428571428</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.830714285</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.89714285714285702</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.93214285714285705</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.94642857142857095</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.98258029526895796</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="5">
+        <v>200</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.42285714285714199</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.495</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.54428571428571404</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.61357142857142799</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.71214285714285697</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.77785714285714203</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.86857142857142799</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.90214285714285702</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.92142857142857104</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.63607165264369803</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="6">
+        <v>300</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.42785714285714199</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.495714285714285</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0.55357142857142805</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.625714285714285</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.71071428571428497</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.79214285714285704</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.86785714285714199</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.89857142857142802</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.91857142857142804</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.77235296856915103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="5">
+        <v>400</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.42428571428571399</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.502857142857142</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0.54857142857142804</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.623571428571428</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.79142857142857104</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.89642857142857102</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.91785714285714204</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.86404662728733195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="5">
+        <v>500</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.41714285714285698</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.498571428571428</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.54785714285714204</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.622142857142857</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.71428571428571397</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.79428569999999998</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.86428571428571399</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.89428571428571402</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.90928571428571403</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.92558005884619998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>